<commit_message>
update README to reflect discord updated calcs
</commit_message>
<xml_diff>
--- a/05 - Projects/Project 01/mesonet xlsx view.xlsx
+++ b/05 - Projects/Project 01/mesonet xlsx view.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbry1\OneDrive\Documents\Github\CS-2334\05 - Projects\Project 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB576DE1-CB01-4029-A782-018D0AB1ED4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EAEF48-4501-45D0-AA9B-F71096F6337D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B867B53B-53BE-4CD0-919A-055D3B5DE54B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B867B53B-53BE-4CD0-919A-055D3B5DE54B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,9 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E3A0A1-2F35-4C6D-9923-2C7CB739C7B0}">
   <dimension ref="B2:J125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -608,22 +606,22 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -632,7 +630,7 @@
       </c>
       <c r="J4" s="4">
         <f>COUNTIF(J6:J125, $J$3)</f>
-        <v>23</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -672,7 +670,7 @@
       </c>
       <c r="H6" s="6">
         <f>IF(D$3 &lt;&gt; D6, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="6">
         <f>IF(E$3 &lt;&gt; E6, 1, 0)</f>
@@ -680,7 +678,7 @@
       </c>
       <c r="J6" s="5">
         <f>SUM(F6:I6)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -872,7 +870,7 @@
       </c>
       <c r="G12" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="2"/>
@@ -884,7 +882,7 @@
       </c>
       <c r="J12" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -906,7 +904,7 @@
       </c>
       <c r="G13" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" si="2"/>
@@ -918,7 +916,7 @@
       </c>
       <c r="J13" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -940,7 +938,7 @@
       </c>
       <c r="G14" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" si="2"/>
@@ -952,7 +950,7 @@
       </c>
       <c r="J14" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -974,7 +972,7 @@
       </c>
       <c r="G15" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="2"/>
@@ -986,7 +984,7 @@
       </c>
       <c r="J15" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -1110,7 +1108,7 @@
       </c>
       <c r="G19" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" si="2"/>
@@ -1122,7 +1120,7 @@
       </c>
       <c r="J19" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -1144,7 +1142,7 @@
       </c>
       <c r="G20" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="6">
         <f t="shared" si="2"/>
@@ -1156,7 +1154,7 @@
       </c>
       <c r="J20" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1178,7 +1176,7 @@
       </c>
       <c r="G21" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" si="2"/>
@@ -1190,7 +1188,7 @@
       </c>
       <c r="J21" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1288,11 +1286,11 @@
       </c>
       <c r="I24" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1356,11 +1354,11 @@
       </c>
       <c r="I26" s="6">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -1386,7 +1384,7 @@
       </c>
       <c r="H27" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="6">
         <f t="shared" si="3"/>
@@ -1394,7 +1392,7 @@
       </c>
       <c r="J27" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -1450,7 +1448,7 @@
       </c>
       <c r="G29" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" si="2"/>
@@ -1462,7 +1460,7 @@
       </c>
       <c r="J29" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -1492,11 +1490,11 @@
       </c>
       <c r="I30" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
@@ -1526,11 +1524,11 @@
       </c>
       <c r="I31" s="6">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1858,7 +1856,7 @@
       </c>
       <c r="G41" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="6">
         <f t="shared" si="2"/>
@@ -1870,7 +1868,7 @@
       </c>
       <c r="J41" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
@@ -1968,11 +1966,11 @@
       </c>
       <c r="I44" s="6">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
@@ -2062,7 +2060,7 @@
       </c>
       <c r="G47" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="6">
         <f t="shared" si="2"/>
@@ -2074,7 +2072,7 @@
       </c>
       <c r="J47" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
@@ -2164,7 +2162,7 @@
       </c>
       <c r="G50" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="6">
         <f t="shared" si="2"/>
@@ -2176,7 +2174,7 @@
       </c>
       <c r="J50" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
@@ -2266,7 +2264,7 @@
       </c>
       <c r="G53" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" s="6">
         <f t="shared" si="2"/>
@@ -2278,7 +2276,7 @@
       </c>
       <c r="J53" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2338,7 +2336,7 @@
       </c>
       <c r="H55" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" s="6">
         <f t="shared" si="3"/>
@@ -2346,7 +2344,7 @@
       </c>
       <c r="J55" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -2606,7 +2604,7 @@
       </c>
       <c r="G63" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" s="6">
         <f t="shared" si="2"/>
@@ -2618,7 +2616,7 @@
       </c>
       <c r="J63" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -2640,7 +2638,7 @@
       </c>
       <c r="G64" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" s="6">
         <f t="shared" si="2"/>
@@ -2652,7 +2650,7 @@
       </c>
       <c r="J64" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -2886,11 +2884,11 @@
       </c>
       <c r="I71" s="6">
         <f t="shared" ref="I71:I125" si="8">IF(E$3 &lt;&gt; E71, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J71" s="5">
         <f t="shared" ref="J71:J125" si="9">SUM(F71:I71)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
@@ -2946,7 +2944,7 @@
       </c>
       <c r="G73" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" s="6">
         <f t="shared" si="7"/>
@@ -2958,7 +2956,7 @@
       </c>
       <c r="J73" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
@@ -2980,7 +2978,7 @@
       </c>
       <c r="G74" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" s="6">
         <f t="shared" si="7"/>
@@ -2992,7 +2990,7 @@
       </c>
       <c r="J74" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -3082,7 +3080,7 @@
       </c>
       <c r="G77" s="6">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H77" s="6">
         <f t="shared" si="7"/>
@@ -3094,7 +3092,7 @@
       </c>
       <c r="J77" s="5">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -3146,11 +3144,11 @@
       </c>
       <c r="F79" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" s="6">
         <f t="shared" si="7"/>
@@ -3180,11 +3178,11 @@
       </c>
       <c r="F80" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G80" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80" s="6">
         <f t="shared" si="7"/>
@@ -3214,7 +3212,7 @@
       </c>
       <c r="F81" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81" s="6">
         <f t="shared" si="6"/>
@@ -3230,7 +3228,7 @@
       </c>
       <c r="J81" s="5">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
@@ -3248,23 +3246,23 @@
       </c>
       <c r="F82" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="6">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" s="6">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I82" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J82" s="5">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
@@ -3392,7 +3390,7 @@
       </c>
       <c r="H86" s="6">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" s="6">
         <f t="shared" si="8"/>
@@ -3400,7 +3398,7 @@
       </c>
       <c r="J86" s="5">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
@@ -3464,11 +3462,11 @@
       </c>
       <c r="I88" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J88" s="5">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
@@ -3490,7 +3488,7 @@
       </c>
       <c r="G89" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89" s="6">
         <f t="shared" si="7"/>
@@ -3502,7 +3500,7 @@
       </c>
       <c r="J89" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
@@ -3558,7 +3556,7 @@
       </c>
       <c r="G91" s="6">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" s="6">
         <f t="shared" si="7"/>
@@ -3570,7 +3568,7 @@
       </c>
       <c r="J91" s="5">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
@@ -3600,11 +3598,11 @@
       </c>
       <c r="I92" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J92" s="5">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
@@ -3626,7 +3624,7 @@
       </c>
       <c r="G93" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93" s="6">
         <f t="shared" si="7"/>
@@ -3634,11 +3632,11 @@
       </c>
       <c r="I93" s="6">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J93" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -3728,7 +3726,7 @@
       </c>
       <c r="G96" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96" s="6">
         <f t="shared" si="7"/>
@@ -3740,7 +3738,7 @@
       </c>
       <c r="J96" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
@@ -3762,11 +3760,11 @@
       </c>
       <c r="G97" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" s="6">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97" s="6">
         <f t="shared" si="8"/>
@@ -3906,11 +3904,11 @@
       </c>
       <c r="I101" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J101" s="5">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
@@ -4246,11 +4244,11 @@
       </c>
       <c r="I111" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111" s="5">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.25">
@@ -4336,7 +4334,7 @@
       </c>
       <c r="F114" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G114" s="6">
         <f t="shared" si="6"/>
@@ -4352,7 +4350,7 @@
       </c>
       <c r="J114" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="2:10" x14ac:dyDescent="0.25">
@@ -4370,7 +4368,7 @@
       </c>
       <c r="F115" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G115" s="6">
         <f t="shared" si="6"/>
@@ -4386,7 +4384,7 @@
       </c>
       <c r="J115" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="2:10" x14ac:dyDescent="0.25">
@@ -4404,7 +4402,7 @@
       </c>
       <c r="F116" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G116" s="6">
         <f t="shared" si="6"/>
@@ -4420,7 +4418,7 @@
       </c>
       <c r="J116" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="2:10" x14ac:dyDescent="0.25">
@@ -4438,7 +4436,7 @@
       </c>
       <c r="F117" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G117" s="6">
         <f t="shared" si="6"/>
@@ -4450,11 +4448,11 @@
       </c>
       <c r="I117" s="6">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J117" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="2:10" x14ac:dyDescent="0.25">
@@ -4472,11 +4470,11 @@
       </c>
       <c r="F118" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G118" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H118" s="6">
         <f t="shared" si="7"/>
@@ -4488,7 +4486,7 @@
       </c>
       <c r="J118" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.25">
@@ -4506,23 +4504,23 @@
       </c>
       <c r="F119" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G119" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H119" s="6">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I119" s="6">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J119" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.25">
@@ -4540,11 +4538,11 @@
       </c>
       <c r="F120" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G120" s="6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H120" s="6">
         <f t="shared" si="7"/>
@@ -4556,7 +4554,7 @@
       </c>
       <c r="J120" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.25">
@@ -4574,7 +4572,7 @@
       </c>
       <c r="F121" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G121" s="6">
         <f t="shared" si="6"/>
@@ -4590,7 +4588,7 @@
       </c>
       <c r="J121" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.25">
@@ -4608,7 +4606,7 @@
       </c>
       <c r="F122" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G122" s="6">
         <f t="shared" si="6"/>
@@ -4624,7 +4622,7 @@
       </c>
       <c r="J122" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="2:10" x14ac:dyDescent="0.25">
@@ -4642,7 +4640,7 @@
       </c>
       <c r="F123" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G123" s="6">
         <f t="shared" si="6"/>
@@ -4658,7 +4656,7 @@
       </c>
       <c r="J123" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="2:10" x14ac:dyDescent="0.25">
@@ -4676,7 +4674,7 @@
       </c>
       <c r="F124" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G124" s="6">
         <f t="shared" si="6"/>
@@ -4692,7 +4690,7 @@
       </c>
       <c r="J124" s="5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>